<commit_message>
updated PM emission factors
</commit_message>
<xml_diff>
--- a/data/figure/regional_optimization_results.xlsx
+++ b/data/figure/regional_optimization_results.xlsx
@@ -585,7 +585,7 @@
         <v>300.0398348807767</v>
       </c>
       <c r="F2">
-        <v>8.727340078635921E-06</v>
+        <v>1.382634065976287E-05</v>
       </c>
       <c r="G2">
         <v>-1.928965070062918</v>
@@ -594,7 +594,7 @@
         <v>13.18265679874991</v>
       </c>
       <c r="I2">
-        <v>3.834475147886557E-07</v>
+        <v>6.07479016153575E-07</v>
       </c>
       <c r="J2">
         <v>1.521368520673843</v>
@@ -644,7 +644,7 @@
         <v>28.09873105856535</v>
       </c>
       <c r="F3">
-        <v>3.654322022554009E-06</v>
+        <v>4.20122047303277E-06</v>
       </c>
       <c r="G3">
         <v>-1.01456247814408</v>
@@ -653,7 +653,7 @@
         <v>3.592904182836322</v>
       </c>
       <c r="I3">
-        <v>4.672676802699556E-07</v>
+        <v>5.371980172028351E-07</v>
       </c>
       <c r="J3">
         <v>2.459991187363163</v>
@@ -703,7 +703,7 @@
         <v>139.9407085384326</v>
       </c>
       <c r="F4">
-        <v>1.701589496317841E-05</v>
+        <v>2.085921004785904E-05</v>
       </c>
       <c r="G4">
         <v>-1.210803187058465</v>
@@ -712,10 +712,10 @@
         <v>6.952047423801463</v>
       </c>
       <c r="I4">
-        <v>8.45324494765958E-07</v>
+        <v>1.036254703797831E-06</v>
       </c>
       <c r="J4">
-        <v>6.197027022450854</v>
+        <v>6.197027022450852</v>
       </c>
       <c r="K4">
         <v>25.32103845776548</v>
@@ -733,7 +733,7 @@
         <v>1.365038917091361</v>
       </c>
       <c r="P4">
-        <v>4.831988105359493</v>
+        <v>4.831988105359491</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -762,7 +762,7 @@
         <v>147.5871783565389</v>
       </c>
       <c r="F5">
-        <v>0.0001269765960542554</v>
+        <v>0.0001548959868376641</v>
       </c>
       <c r="G5">
         <v>0.850327507313936</v>
@@ -771,7 +771,7 @@
         <v>0.679967652781629</v>
       </c>
       <c r="I5">
-        <v>5.850100187472536E-07</v>
+        <v>7.136409935344097E-07</v>
       </c>
       <c r="J5">
         <v>102.8943170985515</v>
@@ -821,7 +821,7 @@
         <v>82.36048841803607</v>
       </c>
       <c r="F6">
-        <v>8.537150457601574E-06</v>
+        <v>1.27401230500977E-05</v>
       </c>
       <c r="G6">
         <v>1.233295303386459</v>
@@ -830,7 +830,7 @@
         <v>1.574363928031817</v>
       </c>
       <c r="I6">
-        <v>1.631921080944549E-07</v>
+        <v>2.435341333450386E-07</v>
       </c>
       <c r="J6">
         <v>20.44623272189754</v>
@@ -880,7 +880,7 @@
         <v>284.145889328476</v>
       </c>
       <c r="F7">
-        <v>3.105620409968406E-05</v>
+        <v>4.378407551380455E-05</v>
       </c>
       <c r="G7">
         <v>0.06003317719794067</v>
@@ -889,7 +889,7 @@
         <v>9.319216934650743</v>
       </c>
       <c r="I7">
-        <v>1.018559528894586E-06</v>
+        <v>1.435999299376044E-06</v>
       </c>
       <c r="J7">
         <v>12.44561808175359</v>
@@ -939,7 +939,7 @@
         <v>326.418013450564</v>
       </c>
       <c r="F8">
-        <v>6.098165106627373E-05</v>
+        <v>9.337651124839381E-05</v>
       </c>
       <c r="G8">
         <v>-0.03038383025741895</v>
@@ -948,7 +948,7 @@
         <v>2.216744633236928</v>
       </c>
       <c r="I8">
-        <v>4.141338472656392E-07</v>
+        <v>6.341313029638098E-07</v>
       </c>
       <c r="J8">
         <v>57.46807198652485</v>
@@ -998,7 +998,7 @@
         <v>33.1406442165317</v>
       </c>
       <c r="F9">
-        <v>9.168324336654531E-06</v>
+        <v>1.465492449052877E-05</v>
       </c>
       <c r="G9">
         <v>1.128332789421589</v>
@@ -1007,7 +1007,7 @@
         <v>1.620061152144971</v>
       </c>
       <c r="I9">
-        <v>4.481882123664333E-07</v>
+        <v>7.163974755469697E-07</v>
       </c>
       <c r="J9">
         <v>10.37069204743402</v>
@@ -1028,7 +1028,7 @@
         <v>5.043835125983811</v>
       </c>
       <c r="P9">
-        <v>5.326856921450205</v>
+        <v>5.326856921450204</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -1057,7 +1057,7 @@
         <v>22.7759305369746</v>
       </c>
       <c r="F10">
-        <v>3.86882092665217E-06</v>
+        <v>6.737137849434186E-06</v>
       </c>
       <c r="G10">
         <v>1.814483394615815</v>
@@ -1066,7 +1066,7 @@
         <v>1.179669408868842</v>
       </c>
       <c r="I10">
-        <v>2.003838959797518E-07</v>
+        <v>3.489471225514912E-07</v>
       </c>
       <c r="J10">
         <v>9.678857511059331</v>
@@ -1116,7 +1116,7 @@
         <v>14.07929525952148</v>
       </c>
       <c r="F11">
-        <v>1.038157774834629E-05</v>
+        <v>1.399606669634641E-05</v>
       </c>
       <c r="G11">
         <v>1.80226518396055</v>
@@ -1125,7 +1125,7 @@
         <v>0.2022889945272324</v>
       </c>
       <c r="I11">
-        <v>1.491607985775445E-07</v>
+        <v>2.010931802446073E-07</v>
       </c>
       <c r="J11">
         <v>31.51081531048448</v>
@@ -1175,7 +1175,7 @@
         <v>137.2554933591605</v>
       </c>
       <c r="F12">
-        <v>6.16082388341287E-06</v>
+        <v>7.54655519551969E-06</v>
       </c>
       <c r="G12">
         <v>0.0825969357974609</v>
@@ -1184,7 +1184,7 @@
         <v>7.190250108071694</v>
       </c>
       <c r="I12">
-        <v>3.227401942857364E-07</v>
+        <v>3.953329515793329E-07</v>
       </c>
       <c r="J12">
         <v>8.703245564278783</v>
@@ -1234,7 +1234,7 @@
         <v>19.55209204214145</v>
       </c>
       <c r="F13">
-        <v>6.688181904610199E-06</v>
+        <v>9.129747256491499E-06</v>
       </c>
       <c r="G13">
         <v>0.4176180281121581</v>
@@ -1243,7 +1243,7 @@
         <v>0.9929952774000489</v>
       </c>
       <c r="I13">
-        <v>3.396737817802845E-07</v>
+        <v>4.636739582655512E-07</v>
       </c>
       <c r="J13">
         <v>8.242554756071838</v>
@@ -1293,7 +1293,7 @@
         <v>67.10892581388435</v>
       </c>
       <c r="F14">
-        <v>8.207113925053162E-08</v>
+        <v>1.85717505888197E-07</v>
       </c>
       <c r="G14">
         <v>-0.9549086199246515</v>
@@ -1302,7 +1302,7 @@
         <v>9.24152516251722</v>
       </c>
       <c r="I14">
-        <v>1.130196153941898E-08</v>
+        <v>2.557503317137912E-08</v>
       </c>
       <c r="J14">
         <v>3.284968803621055</v>
@@ -1352,7 +1352,7 @@
         <v>109.4579665327152</v>
       </c>
       <c r="F15">
-        <v>4.379071063853281E-06</v>
+        <v>5.262356315591319E-06</v>
       </c>
       <c r="G15">
         <v>0.300430341598808</v>
@@ -1361,7 +1361,7 @@
         <v>8.676271735253682</v>
       </c>
       <c r="I15">
-        <v>3.471105091891296E-07</v>
+        <v>4.171248088018548E-07</v>
       </c>
       <c r="J15">
         <v>5.525804960008053</v>
@@ -1411,7 +1411,7 @@
         <v>68.44639451210084</v>
       </c>
       <c r="F16">
-        <v>1.76496427658026E-06</v>
+        <v>2.258412964584752E-06</v>
       </c>
       <c r="G16">
         <v>-0.8719457639206813</v>
@@ -1420,7 +1420,7 @@
         <v>10.48508847120711</v>
       </c>
       <c r="I16">
-        <v>2.703693411519635E-07</v>
+        <v>3.459591978070643E-07</v>
       </c>
       <c r="J16">
         <v>2.467725778877002</v>
@@ -1470,7 +1470,7 @@
         <v>288.9101677983943</v>
       </c>
       <c r="F17">
-        <v>3.657003059411093E-06</v>
+        <v>6.475866766200601E-06</v>
       </c>
       <c r="G17">
         <v>-1.557243674187316</v>
@@ -1479,7 +1479,7 @@
         <v>10.79074028417718</v>
       </c>
       <c r="I17">
-        <v>1.365883746261345E-07</v>
+        <v>2.418724024893712E-07</v>
       </c>
       <c r="J17">
         <v>7.878728355435905</v>
@@ -1529,7 +1529,7 @@
         <v>95.60671934865732</v>
       </c>
       <c r="F18">
-        <v>3.21599987580003E-05</v>
+        <v>4.288963697973602E-05</v>
       </c>
       <c r="G18">
         <v>-1.494798550500435</v>
@@ -1538,7 +1538,7 @@
         <v>5.279553430344471</v>
       </c>
       <c r="I18">
-        <v>1.77592571860441E-06</v>
+        <v>2.368433218765961E-06</v>
       </c>
       <c r="J18">
         <v>1.721629730573583</v>
@@ -1588,7 +1588,7 @@
         <v>23.51615830755628</v>
       </c>
       <c r="F19">
-        <v>3.436550938084094E-06</v>
+        <v>5.635905489433516E-06</v>
       </c>
       <c r="G19">
         <v>-0.6614516029185383</v>
@@ -1597,10 +1597,10 @@
         <v>1.146816288478698</v>
       </c>
       <c r="I19">
-        <v>1.67590834371753E-07</v>
+        <v>2.748471128267598E-07</v>
       </c>
       <c r="J19">
-        <v>7.247299826271891</v>
+        <v>7.24729982627189</v>
       </c>
       <c r="K19">
         <v>13.22621825674478</v>
@@ -1618,7 +1618,7 @@
         <v>2.28872265370742</v>
       </c>
       <c r="P19">
-        <v>4.958577172564471</v>
+        <v>4.95857717256447</v>
       </c>
       <c r="Q19">
         <v>0.9999999809556833</v>
@@ -1647,7 +1647,7 @@
         <v>567.3391188268197</v>
       </c>
       <c r="F20">
-        <v>3.088025864353377E-05</v>
+        <v>4.392059431836404E-05</v>
       </c>
       <c r="G20">
         <v>-0.250206538366956</v>
@@ -1656,7 +1656,7 @@
         <v>10.2795994650679</v>
       </c>
       <c r="I20">
-        <v>5.595184250464593E-07</v>
+        <v>7.957958527417099E-07</v>
       </c>
       <c r="J20">
         <v>23.33051146479145</v>
@@ -1706,7 +1706,7 @@
         <v>16.53368543345142</v>
       </c>
       <c r="F21">
-        <v>1.886115938609777E-06</v>
+        <v>2.163948326237687E-06</v>
       </c>
       <c r="G21">
         <v>0.1400882113544724</v>
@@ -1715,7 +1715,7 @@
         <v>2.207420204470063</v>
       </c>
       <c r="I21">
-        <v>2.51816235866967E-07</v>
+        <v>2.889097700565782E-07</v>
       </c>
       <c r="J21">
         <v>3.203290893119632</v>
@@ -1765,7 +1765,7 @@
         <v>57.91067190174348</v>
       </c>
       <c r="F22">
-        <v>9.54738996016019E-06</v>
+        <v>1.058311753997767E-05</v>
       </c>
       <c r="G22">
         <v>0.8177853439729809</v>
@@ -1774,7 +1774,7 @@
         <v>4.317600333896884</v>
       </c>
       <c r="I22">
-        <v>7.118172303331599E-07</v>
+        <v>7.890371553934932E-07</v>
       </c>
       <c r="J22">
         <v>6.189369749352442</v>
@@ -1821,7 +1821,7 @@
         <v>28.97038664112452</v>
       </c>
       <c r="F23">
-        <v>4.111688644393109E-06</v>
+        <v>4.893818013976255E-06</v>
       </c>
       <c r="G23">
         <v>-1.307050985526581</v>
@@ -1830,7 +1830,7 @@
         <v>5.843007037164541</v>
       </c>
       <c r="I23">
-        <v>8.292821901698278E-07</v>
+        <v>9.870290461941837E-07</v>
       </c>
       <c r="J23">
         <v>1.430858248763794</v>
@@ -1880,7 +1880,7 @@
         <v>391.462736689382</v>
       </c>
       <c r="F24">
-        <v>2.554614703989987E-05</v>
+        <v>3.360011278728484E-05</v>
       </c>
       <c r="G24">
         <v>-1.273934632347765</v>
@@ -1889,7 +1889,7 @@
         <v>4.818668151472752</v>
       </c>
       <c r="I24">
-        <v>3.144575296618375E-07</v>
+        <v>4.135969485710015E-07</v>
       </c>
       <c r="J24">
         <v>30.36557155018749</v>
@@ -1939,7 +1939,7 @@
         <v>147.5017939624075</v>
       </c>
       <c r="F25">
-        <v>4.612390434525096E-06</v>
+        <v>8.471606196148185E-06</v>
       </c>
       <c r="G25">
         <v>-1.877033839546842</v>
@@ -1948,7 +1948,7 @@
         <v>7.670678094004245</v>
       </c>
       <c r="I25">
-        <v>2.398625895772047E-07</v>
+        <v>4.405571100130901E-07</v>
       </c>
       <c r="J25">
         <v>1.701044332696608</v>
@@ -1969,7 +1969,7 @@
         <v>1.151944300299625</v>
       </c>
       <c r="P25">
-        <v>0.5491000323969828</v>
+        <v>0.549100032396983</v>
       </c>
       <c r="Q25">
         <v>1</v>
@@ -1998,7 +1998,7 @@
         <v>390.4351971113464</v>
       </c>
       <c r="F26">
-        <v>6.601191881851058E-05</v>
+        <v>7.801397553460706E-05</v>
       </c>
       <c r="G26">
         <v>-0.153899007437803</v>
@@ -2007,10 +2007,10 @@
         <v>4.800551495940617</v>
       </c>
       <c r="I26">
-        <v>8.116420291476388E-07</v>
+        <v>9.592119504792695E-07</v>
       </c>
       <c r="J26">
-        <v>39.21564912698201</v>
+        <v>39.21564912698202</v>
       </c>
       <c r="K26">
         <v>46.1855034696796</v>
@@ -2057,7 +2057,7 @@
         <v>4233.659208746598</v>
       </c>
       <c r="F27">
-        <v>0.0005183207841234918</v>
+        <v>0.0007128246121174162</v>
       </c>
       <c r="G27">
         <v>-0.2530288055688681</v>
@@ -2066,7 +2066,7 @@
         <v>4.204045321707362</v>
       </c>
       <c r="I27">
-        <v>5.146951986915303E-07</v>
+        <v>7.07838498096141E-07</v>
       </c>
       <c r="J27">
         <v>453.4737409605383</v>
@@ -2087,7 +2087,7 @@
         <v>221.3737946220806</v>
       </c>
       <c r="P27">
-        <v>232.0999463384576</v>
+        <v>232.0999463384577</v>
       </c>
       <c r="Q27">
         <v>1</v>
@@ -2116,7 +2116,7 @@
         <v>69.10888659389632</v>
       </c>
       <c r="F28">
-        <v>1.059102691691112E-06</v>
+        <v>1.42737863519668E-06</v>
       </c>
       <c r="G28">
         <v>-1.348819095244547</v>
@@ -2125,7 +2125,7 @@
         <v>10.72872221729807</v>
       </c>
       <c r="I28">
-        <v>1.64419065894055E-07</v>
+        <v>2.215916017562312E-07</v>
       </c>
       <c r="J28">
         <v>2.809371202505648</v>

</xml_diff>